<commit_message>
EPBDS-8248 support StringRange in SmartRules and SimpleRules
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Ranges_StringRange.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Ranges_StringRange.xlsx
@@ -3,12 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0EC2C0-09AF-49C7-A114-865DF45E4542}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC854FF-3F84-48CD-AB9B-EE5B00CAF369}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="3" r:id="rId1"/>
+    <sheet name="SmartRules" sheetId="4" r:id="rId2"/>
+    <sheet name="SimpleRules" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="107">
   <si>
     <t>d</t>
   </si>
@@ -124,9 +126,6 @@
     <t>Empty</t>
   </si>
   <si>
-    <t>Rules String Rules_StringRangeMinMax(String d)</t>
-  </si>
-  <si>
     <t>AAA-DD</t>
   </si>
   <si>
@@ -163,9 +162,6 @@
     <t>ZZZZZY</t>
   </si>
   <si>
-    <t>Rules String Rules_StringRangeBrackets(String d)</t>
-  </si>
-  <si>
     <t>[AAA; DD]</t>
   </si>
   <si>
@@ -305,6 +301,48 @@
   </si>
   <si>
     <t>Test Rules_StringRangeMoreLess2</t>
+  </si>
+  <si>
+    <t>SimpleRules String SimpleRules_StringRangeBrackets(String d)</t>
+  </si>
+  <si>
+    <t>AAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>AAAA - BBBB</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>LML  … VVVV</t>
+  </si>
+  <si>
+    <t>Test SimpleRules_StringRangeBrackets</t>
+  </si>
+  <si>
+    <t>AAAAA</t>
+  </si>
+  <si>
+    <t>BBBB</t>
+  </si>
+  <si>
+    <t>BBBBB</t>
+  </si>
+  <si>
+    <t>SmartRules String SmartRules_StringRangeBrackets(String d)</t>
+  </si>
+  <si>
+    <t>Test SmartRules_StringRangeBrackets</t>
+  </si>
+  <si>
+    <t>Rules String Rules_StringRangeMinMax(StringValue d)</t>
+  </si>
+  <si>
+    <t>Rules String Rules_StringRangeBrackets(StringValue d)</t>
   </si>
 </sst>
 </file>
@@ -712,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B702F4-5B69-4EC8-A5A1-B560C84EFEE3}">
   <dimension ref="B2:D276"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -972,7 +1010,7 @@
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="8" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="C40" s="8"/>
     </row>
@@ -1010,7 +1048,7 @@
     </row>
     <row r="45" spans="2:4">
       <c r="B45" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>2</v>
@@ -1026,7 +1064,7 @@
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>13</v>
@@ -1034,7 +1072,7 @@
     </row>
     <row r="48" spans="2:4">
       <c r="B48" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>4</v>
@@ -1042,7 +1080,7 @@
     </row>
     <row r="52" spans="2:4">
       <c r="B52" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
@@ -1106,7 +1144,7 @@
     <row r="59" spans="2:4">
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>2</v>
@@ -1160,7 +1198,7 @@
     <row r="65" spans="2:4">
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>4</v>
@@ -1169,7 +1207,7 @@
     <row r="66" spans="2:4">
       <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>4</v>
@@ -1178,7 +1216,7 @@
     <row r="67" spans="2:4">
       <c r="B67" s="1"/>
       <c r="C67" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>4</v>
@@ -1187,7 +1225,7 @@
     <row r="68" spans="2:4">
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>4</v>
@@ -1214,7 +1252,7 @@
     <row r="71" spans="2:4">
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>13</v>
@@ -1223,20 +1261,20 @@
     <row r="72" spans="2:4">
       <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D72" s="1"/>
     </row>
     <row r="73" spans="2:4">
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D73" s="1"/>
     </row>
     <row r="77" spans="2:4">
       <c r="B77" s="8" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="C77" s="8"/>
     </row>
@@ -1274,7 +1312,7 @@
     </row>
     <row r="82" spans="2:4">
       <c r="B82" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>2</v>
@@ -1282,7 +1320,7 @@
     </row>
     <row r="83" spans="2:4">
       <c r="B83" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>3</v>
@@ -1290,7 +1328,7 @@
     </row>
     <row r="84" spans="2:4">
       <c r="B84" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>4</v>
@@ -1298,7 +1336,7 @@
     </row>
     <row r="85" spans="2:4">
       <c r="B85" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>13</v>
@@ -1306,7 +1344,7 @@
     </row>
     <row r="89" spans="2:4">
       <c r="B89" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
@@ -1368,7 +1406,7 @@
     <row r="96" spans="2:4">
       <c r="B96" s="1"/>
       <c r="C96" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>2</v>
@@ -1377,7 +1415,7 @@
     <row r="97" spans="2:4">
       <c r="B97" s="1"/>
       <c r="C97" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>3</v>
@@ -1386,7 +1424,7 @@
     <row r="98" spans="2:4">
       <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>3</v>
@@ -1395,7 +1433,7 @@
     <row r="99" spans="2:4">
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>4</v>
@@ -1404,7 +1442,7 @@
     <row r="100" spans="2:4">
       <c r="B100" s="1"/>
       <c r="C100" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>3</v>
@@ -1413,7 +1451,7 @@
     <row r="101" spans="2:4">
       <c r="B101" s="1"/>
       <c r="C101" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>4</v>
@@ -1422,7 +1460,7 @@
     <row r="102" spans="2:4">
       <c r="B102" s="1"/>
       <c r="C102" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>13</v>
@@ -1431,14 +1469,14 @@
     <row r="103" spans="2:4">
       <c r="B103" s="1"/>
       <c r="C103" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D103" s="1"/>
     </row>
     <row r="104" spans="2:4">
       <c r="B104" s="1"/>
       <c r="C104" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>13</v>
@@ -1447,13 +1485,13 @@
     <row r="105" spans="2:4">
       <c r="B105" s="1"/>
       <c r="C105" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D105" s="1"/>
     </row>
     <row r="109" spans="2:4">
       <c r="B109" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C109" s="8"/>
     </row>
@@ -1491,7 +1529,7 @@
     </row>
     <row r="114" spans="2:4">
       <c r="B114" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>2</v>
@@ -1499,7 +1537,7 @@
     </row>
     <row r="115" spans="2:4">
       <c r="B115" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>3</v>
@@ -1507,7 +1545,7 @@
     </row>
     <row r="116" spans="2:4">
       <c r="B116" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>4</v>
@@ -1515,7 +1553,7 @@
     </row>
     <row r="117" spans="2:4">
       <c r="B117" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>13</v>
@@ -1523,7 +1561,7 @@
     </row>
     <row r="120" spans="2:4">
       <c r="B120" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
@@ -1585,7 +1623,7 @@
     <row r="127" spans="2:4">
       <c r="B127" s="1"/>
       <c r="C127" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>2</v>
@@ -1594,7 +1632,7 @@
     <row r="128" spans="2:4">
       <c r="B128" s="1"/>
       <c r="C128" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>3</v>
@@ -1603,7 +1641,7 @@
     <row r="129" spans="2:4">
       <c r="B129" s="1"/>
       <c r="C129" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>3</v>
@@ -1612,7 +1650,7 @@
     <row r="130" spans="2:4">
       <c r="B130" s="1"/>
       <c r="C130" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>4</v>
@@ -1621,7 +1659,7 @@
     <row r="131" spans="2:4">
       <c r="B131" s="1"/>
       <c r="C131" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>3</v>
@@ -1630,7 +1668,7 @@
     <row r="132" spans="2:4">
       <c r="B132" s="1"/>
       <c r="C132" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>4</v>
@@ -1639,7 +1677,7 @@
     <row r="133" spans="2:4">
       <c r="B133" s="1"/>
       <c r="C133" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>13</v>
@@ -1648,14 +1686,14 @@
     <row r="134" spans="2:4">
       <c r="B134" s="1"/>
       <c r="C134" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D134" s="1"/>
     </row>
     <row r="135" spans="2:4">
       <c r="B135" s="1"/>
       <c r="C135" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>13</v>
@@ -1664,13 +1702,13 @@
     <row r="136" spans="2:4">
       <c r="B136" s="1"/>
       <c r="C136" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D136" s="1"/>
     </row>
     <row r="140" spans="2:4">
       <c r="B140" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C140" s="8"/>
     </row>
@@ -1708,7 +1746,7 @@
     </row>
     <row r="145" spans="2:4">
       <c r="B145" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C145" s="7" t="s">
         <v>2</v>
@@ -1716,7 +1754,7 @@
     </row>
     <row r="146" spans="2:4">
       <c r="B146" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>3</v>
@@ -1724,7 +1762,7 @@
     </row>
     <row r="147" spans="2:4">
       <c r="B147" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C147" s="7" t="s">
         <v>4</v>
@@ -1732,7 +1770,7 @@
     </row>
     <row r="148" spans="2:4">
       <c r="B148" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C148" s="7" t="s">
         <v>13</v>
@@ -1740,7 +1778,7 @@
     </row>
     <row r="151" spans="2:4">
       <c r="B151" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
@@ -1802,7 +1840,7 @@
     <row r="158" spans="2:4">
       <c r="B158" s="1"/>
       <c r="C158" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>2</v>
@@ -1811,7 +1849,7 @@
     <row r="159" spans="2:4">
       <c r="B159" s="1"/>
       <c r="C159" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>3</v>
@@ -1820,7 +1858,7 @@
     <row r="160" spans="2:4">
       <c r="B160" s="1"/>
       <c r="C160" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>3</v>
@@ -1829,7 +1867,7 @@
     <row r="161" spans="2:4">
       <c r="B161" s="1"/>
       <c r="C161" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D161" s="1" t="s">
         <v>4</v>
@@ -1838,7 +1876,7 @@
     <row r="162" spans="2:4">
       <c r="B162" s="1"/>
       <c r="C162" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D162" s="1" t="s">
         <v>3</v>
@@ -1847,7 +1885,7 @@
     <row r="163" spans="2:4">
       <c r="B163" s="1"/>
       <c r="C163" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>4</v>
@@ -1856,7 +1894,7 @@
     <row r="164" spans="2:4">
       <c r="B164" s="1"/>
       <c r="C164" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>13</v>
@@ -1865,14 +1903,14 @@
     <row r="165" spans="2:4">
       <c r="B165" s="1"/>
       <c r="C165" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D165" s="1"/>
     </row>
     <row r="166" spans="2:4">
       <c r="B166" s="1"/>
       <c r="C166" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>13</v>
@@ -1881,13 +1919,13 @@
     <row r="167" spans="2:4">
       <c r="B167" s="1"/>
       <c r="C167" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D167" s="1"/>
     </row>
     <row r="172" spans="2:4">
       <c r="B172" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C172" s="8"/>
     </row>
@@ -1925,7 +1963,7 @@
     </row>
     <row r="177" spans="2:4">
       <c r="B177" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C177" s="7" t="s">
         <v>2</v>
@@ -1933,7 +1971,7 @@
     </row>
     <row r="178" spans="2:4">
       <c r="B178" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C178" s="7" t="s">
         <v>3</v>
@@ -1941,7 +1979,7 @@
     </row>
     <row r="179" spans="2:4">
       <c r="B179" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C179" s="7" t="s">
         <v>4</v>
@@ -1949,7 +1987,7 @@
     </row>
     <row r="180" spans="2:4">
       <c r="B180" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C180" s="7" t="s">
         <v>13</v>
@@ -1957,7 +1995,7 @@
     </row>
     <row r="183" spans="2:4">
       <c r="B183" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C183" s="8"/>
       <c r="D183" s="8"/>
@@ -2021,7 +2059,7 @@
     <row r="190" spans="2:4">
       <c r="B190" s="1"/>
       <c r="C190" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>3</v>
@@ -2039,7 +2077,7 @@
     <row r="192" spans="2:4">
       <c r="B192" s="1"/>
       <c r="C192" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D192" s="1" t="s">
         <v>3</v>
@@ -2048,7 +2086,7 @@
     <row r="193" spans="2:4">
       <c r="B193" s="1"/>
       <c r="C193" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D193" s="1" t="s">
         <v>3</v>
@@ -2057,14 +2095,14 @@
     <row r="194" spans="2:4">
       <c r="B194" s="1"/>
       <c r="C194" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D194" s="1"/>
     </row>
     <row r="195" spans="2:4">
       <c r="B195" s="1"/>
       <c r="C195" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D195" s="1"/>
     </row>
@@ -2154,7 +2192,7 @@
     </row>
     <row r="209" spans="2:4">
       <c r="B209" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C209" s="8"/>
     </row>
@@ -2192,7 +2230,7 @@
     </row>
     <row r="214" spans="2:4">
       <c r="B214" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C214" s="7" t="s">
         <v>2</v>
@@ -2200,7 +2238,7 @@
     </row>
     <row r="215" spans="2:4">
       <c r="B215" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C215" s="7" t="s">
         <v>3</v>
@@ -2208,7 +2246,7 @@
     </row>
     <row r="216" spans="2:4">
       <c r="B216" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C216" s="7" t="s">
         <v>4</v>
@@ -2216,7 +2254,7 @@
     </row>
     <row r="217" spans="2:4">
       <c r="B217" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C217" s="7" t="s">
         <v>13</v>
@@ -2224,7 +2262,7 @@
     </row>
     <row r="220" spans="2:4">
       <c r="B220" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C220" s="8"/>
       <c r="D220" s="8"/>
@@ -2288,7 +2326,7 @@
     <row r="227" spans="2:4">
       <c r="B227" s="1"/>
       <c r="C227" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D227" s="1" t="s">
         <v>3</v>
@@ -2306,7 +2344,7 @@
     <row r="229" spans="2:4">
       <c r="B229" s="1"/>
       <c r="C229" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D229" s="1" t="s">
         <v>3</v>
@@ -2315,7 +2353,7 @@
     <row r="230" spans="2:4">
       <c r="B230" s="1"/>
       <c r="C230" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D230" s="1" t="s">
         <v>3</v>
@@ -2324,14 +2362,14 @@
     <row r="231" spans="2:4">
       <c r="B231" s="1"/>
       <c r="C231" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D231" s="1"/>
     </row>
     <row r="232" spans="2:4">
       <c r="B232" s="1"/>
       <c r="C232" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D232" s="1"/>
     </row>
@@ -2421,7 +2459,7 @@
     </row>
     <row r="245" spans="2:4">
       <c r="B245" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C245" s="8"/>
     </row>
@@ -2459,7 +2497,7 @@
     </row>
     <row r="250" spans="2:4">
       <c r="B250" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C250" s="7" t="s">
         <v>2</v>
@@ -2467,7 +2505,7 @@
     </row>
     <row r="254" spans="2:4">
       <c r="B254" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C254" s="8"/>
       <c r="D254" s="8"/>
@@ -2527,7 +2565,7 @@
     <row r="261" spans="2:4">
       <c r="B261" s="1"/>
       <c r="C261" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D261" s="1" t="s">
         <v>2</v>
@@ -2545,7 +2583,7 @@
     <row r="263" spans="2:4">
       <c r="B263" s="1"/>
       <c r="C263" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D263" s="1" t="s">
         <v>2</v>
@@ -2554,7 +2592,7 @@
     <row r="264" spans="2:4">
       <c r="B264" s="1"/>
       <c r="C264" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D264" s="1" t="s">
         <v>2</v>
@@ -2563,7 +2601,7 @@
     <row r="265" spans="2:4">
       <c r="B265" s="1"/>
       <c r="C265" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D265" s="1" t="s">
         <v>2</v>
@@ -2572,7 +2610,7 @@
     <row r="266" spans="2:4">
       <c r="B266" s="1"/>
       <c r="C266" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D266" s="1" t="s">
         <v>2</v>
@@ -2690,4 +2728,596 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C9281C-93D8-4A0A-B8A9-03B437591C0A}">
+  <dimension ref="B3:D36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4">
+      <c r="B3" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B13:D13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7E3F51-50BC-4343-9373-4CD61810EE9B}">
+  <dimension ref="B2:D37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4">
+      <c r="B2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B14:D14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-8248 Add test for StringRange in Spreadsheat
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Ranges_StringRange.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Ranges_StringRange.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC854FF-3F84-48CD-AB9B-EE5B00CAF369}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="3" r:id="rId1"/>
     <sheet name="SmartRules" sheetId="4" r:id="rId2"/>
     <sheet name="SimpleRules" sheetId="5" r:id="rId3"/>
+    <sheet name="Spreadsheet" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="135">
   <si>
     <t>d</t>
   </si>
@@ -343,13 +343,97 @@
   </si>
   <si>
     <t>Rules String Rules_StringRangeBrackets(StringValue d)</t>
+  </si>
+  <si>
+    <t>00F-00Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steps </t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Step1</t>
+  </si>
+  <si>
+    <t>Step2</t>
+  </si>
+  <si>
+    <t>Step3</t>
+  </si>
+  <si>
+    <t>Constants</t>
+  </si>
+  <si>
+    <t>StringRange</t>
+  </si>
+  <si>
+    <t>&lt;AAA</t>
+  </si>
+  <si>
+    <t>range4</t>
+  </si>
+  <si>
+    <t>range5</t>
+  </si>
+  <si>
+    <t>=range5</t>
+  </si>
+  <si>
+    <t>more than Z</t>
+  </si>
+  <si>
+    <t>=$Step1 .contains(a)</t>
+  </si>
+  <si>
+    <t>=b .contains(a)</t>
+  </si>
+  <si>
+    <t>Step4</t>
+  </si>
+  <si>
+    <t>=b==range4</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>_res_.$Value$Step1</t>
+  </si>
+  <si>
+    <t>_res_.$Value$Step2</t>
+  </si>
+  <si>
+    <t>_res_.$Value$Step3</t>
+  </si>
+  <si>
+    <t>_res_.$Value$Step4</t>
+  </si>
+  <si>
+    <t>Test Spreadsheet_stringRange Spreadsheet_stringRangeTest</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult Spreadsheet_stringRange(String a, StringRange b)</t>
+  </si>
+  <si>
+    <t>&gt;Z</t>
+  </si>
+  <si>
+    <t>less than AAA</t>
+  </si>
+  <si>
+    <t>[C..D]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,16 +452,8 @@
       <color indexed="8"/>
       <name val="&quot;Franklin Gothik Book&quot;"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="186"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,8 +492,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -440,12 +528,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -467,13 +591,52 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="1" xr:uid="{419CB39F-E099-4E74-8BFD-D479D4946710}"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -740,25 +903,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B702F4-5B69-4EC8-A5A1-B560C84EFEE3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B77" sqref="B77:C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -825,7 +988,7 @@
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="6" t="s">
-        <v>16</v>
+        <v>107</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>13</v>
@@ -2731,7 +2894,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C9281C-93D8-4A0A-B8A9-03B437591C0A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2740,9 +2903,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4">
@@ -3027,7 +3190,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7E3F51-50BC-4343-9373-4CD61810EE9B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3036,9 +3199,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -3320,4 +3483,189 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:L17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:12">
+      <c r="B4" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="G4" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="B16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="G4:L4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-8323 Simple Rules incorrectly understands if Range or Array in in condition for Range datatypes
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Ranges_StringRange.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Ranges_StringRange.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478187BA-31E1-4645-975D-FD216082B648}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
+    <workbookView xWindow="4425" yWindow="1290" windowWidth="31485" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="3" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="135">
   <si>
     <t>d</t>
   </si>
@@ -432,7 +433,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -588,10 +589,12 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -601,11 +604,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -632,7 +633,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -903,18 +904,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:D276"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B77" sqref="B77:C85"/>
+    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -925,10 +926,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="3" t="s">
@@ -995,11 +996,11 @@
       </c>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="2" t="s">
@@ -1062,9 +1063,7 @@
       <c r="C21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="1"/>
@@ -1172,10 +1171,10 @@
       <c r="D36" s="1"/>
     </row>
     <row r="40" spans="2:4">
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C40" s="8"/>
+      <c r="C40" s="11"/>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="3" t="s">
@@ -1242,11 +1241,11 @@
       </c>
     </row>
     <row r="52" spans="2:4">
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
     </row>
     <row r="53" spans="2:4">
       <c r="B53" s="2" t="s">
@@ -1436,10 +1435,10 @@
       <c r="D73" s="1"/>
     </row>
     <row r="77" spans="2:4">
-      <c r="B77" s="8" t="s">
+      <c r="B77" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C77" s="8"/>
+      <c r="C77" s="11"/>
     </row>
     <row r="78" spans="2:4">
       <c r="B78" s="3" t="s">
@@ -1506,11 +1505,11 @@
       </c>
     </row>
     <row r="89" spans="2:4">
-      <c r="B89" s="8" t="s">
+      <c r="B89" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
     </row>
     <row r="90" spans="2:4">
       <c r="B90" s="2" t="s">
@@ -1653,10 +1652,10 @@
       <c r="D105" s="1"/>
     </row>
     <row r="109" spans="2:4">
-      <c r="B109" s="8" t="s">
+      <c r="B109" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C109" s="8"/>
+      <c r="C109" s="11"/>
     </row>
     <row r="110" spans="2:4">
       <c r="B110" s="3" t="s">
@@ -1723,11 +1722,11 @@
       </c>
     </row>
     <row r="120" spans="2:4">
-      <c r="B120" s="8" t="s">
+      <c r="B120" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C120" s="8"/>
-      <c r="D120" s="8"/>
+      <c r="C120" s="11"/>
+      <c r="D120" s="11"/>
     </row>
     <row r="121" spans="2:4">
       <c r="B121" s="2" t="s">
@@ -1870,10 +1869,10 @@
       <c r="D136" s="1"/>
     </row>
     <row r="140" spans="2:4">
-      <c r="B140" s="8" t="s">
+      <c r="B140" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C140" s="8"/>
+      <c r="C140" s="11"/>
     </row>
     <row r="141" spans="2:4">
       <c r="B141" s="3" t="s">
@@ -1940,11 +1939,11 @@
       </c>
     </row>
     <row r="151" spans="2:4">
-      <c r="B151" s="8" t="s">
+      <c r="B151" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C151" s="8"/>
-      <c r="D151" s="8"/>
+      <c r="C151" s="11"/>
+      <c r="D151" s="11"/>
     </row>
     <row r="152" spans="2:4">
       <c r="B152" s="2" t="s">
@@ -2087,10 +2086,10 @@
       <c r="D167" s="1"/>
     </row>
     <row r="172" spans="2:4">
-      <c r="B172" s="8" t="s">
+      <c r="B172" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C172" s="8"/>
+      <c r="C172" s="11"/>
     </row>
     <row r="173" spans="2:4">
       <c r="B173" s="3" t="s">
@@ -2157,11 +2156,11 @@
       </c>
     </row>
     <row r="183" spans="2:4">
-      <c r="B183" s="8" t="s">
+      <c r="B183" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C183" s="8"/>
-      <c r="D183" s="8"/>
+      <c r="C183" s="11"/>
+      <c r="D183" s="11"/>
     </row>
     <row r="184" spans="2:4">
       <c r="B184" s="2" t="s">
@@ -2354,10 +2353,10 @@
       </c>
     </row>
     <row r="209" spans="2:4">
-      <c r="B209" s="8" t="s">
+      <c r="B209" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C209" s="8"/>
+      <c r="C209" s="11"/>
     </row>
     <row r="210" spans="2:4">
       <c r="B210" s="3" t="s">
@@ -2424,11 +2423,11 @@
       </c>
     </row>
     <row r="220" spans="2:4">
-      <c r="B220" s="8" t="s">
+      <c r="B220" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C220" s="8"/>
-      <c r="D220" s="8"/>
+      <c r="C220" s="11"/>
+      <c r="D220" s="11"/>
     </row>
     <row r="221" spans="2:4">
       <c r="B221" s="2" t="s">
@@ -2621,10 +2620,10 @@
       </c>
     </row>
     <row r="245" spans="2:4">
-      <c r="B245" s="8" t="s">
+      <c r="B245" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C245" s="8"/>
+      <c r="C245" s="11"/>
     </row>
     <row r="246" spans="2:4">
       <c r="B246" s="3" t="s">
@@ -2667,11 +2666,11 @@
       </c>
     </row>
     <row r="254" spans="2:4">
-      <c r="B254" s="8" t="s">
+      <c r="B254" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C254" s="8"/>
-      <c r="D254" s="8"/>
+      <c r="C254" s="11"/>
+      <c r="D254" s="11"/>
     </row>
     <row r="255" spans="2:4">
       <c r="B255" s="2" t="s">
@@ -2894,7 +2893,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2909,10 +2908,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="4" t="s">
@@ -2971,11 +2970,11 @@
       </c>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="2" t="s">
@@ -3190,10 +3189,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -3205,10 +3204,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="4" t="s">
@@ -3267,11 +3266,11 @@
       </c>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="2" t="s">
@@ -3486,10 +3485,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B4:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -3506,24 +3505,24 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:12">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="G4" s="8" t="s">
+      <c r="C4" s="11"/>
+      <c r="G4" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="10" t="s">
         <v>109</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -3549,7 +3548,7 @@
       <c r="B6" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>118</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -3575,7 +3574,7 @@
       <c r="B7" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>120</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -3601,7 +3600,7 @@
       <c r="B8" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>121</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -3627,16 +3626,16 @@
       <c r="B9" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="2:12">
       <c r="B16" s="1" t="s">

</xml_diff>

<commit_message>
EPBDS-8633 Add additionl tests
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Ranges_StringRange.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Ranges_StringRange.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478187BA-31E1-4645-975D-FD216082B648}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4425" yWindow="1290" windowWidth="31485" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4425" yWindow="1290" windowWidth="31485" windowHeight="15300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="3" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="219">
   <si>
     <t>d</t>
   </si>
@@ -169,9 +168,6 @@
     <t>(DD .. FFF]</t>
   </si>
   <si>
-    <t>[FFG; LMM)</t>
-  </si>
-  <si>
     <t>(LML; VVVV)</t>
   </si>
   <si>
@@ -428,13 +424,268 @@
   </si>
   <si>
     <t>[C..D]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EK1</t>
+  </si>
+  <si>
+    <t>WAAAAAAAAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WAAAAAAAAC </t>
+  </si>
+  <si>
+    <t>EK2</t>
+  </si>
+  <si>
+    <t>WWWZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EK2</t>
+  </si>
+  <si>
+    <t>more than     WWW</t>
+  </si>
+  <si>
+    <t>EK3</t>
+  </si>
+  <si>
+    <t>(Z1..Z3)</t>
+  </si>
+  <si>
+    <t>Z2</t>
+  </si>
+  <si>
+    <t>[Z4..Z5]</t>
+  </si>
+  <si>
+    <t>EK4</t>
+  </si>
+  <si>
+    <t>Z5</t>
+  </si>
+  <si>
+    <t>EK5</t>
+  </si>
+  <si>
+    <t>Z6</t>
+  </si>
+  <si>
+    <t>[  Z6  ;   Z7  )</t>
+  </si>
+  <si>
+    <t>[FFG;LMM)</t>
+  </si>
+  <si>
+    <t>[  Z8  ..  Z9  ]</t>
+  </si>
+  <si>
+    <t>EK6</t>
+  </si>
+  <si>
+    <t>Z9</t>
+  </si>
+  <si>
+    <t>EK7</t>
+  </si>
+  <si>
+    <t>Z10  -  Z12</t>
+  </si>
+  <si>
+    <t>Z12</t>
+  </si>
+  <si>
+    <t>Z13..Z15</t>
+  </si>
+  <si>
+    <t>EK8</t>
+  </si>
+  <si>
+    <t>Z15</t>
+  </si>
+  <si>
+    <t>Z17 ..  Z19</t>
+  </si>
+  <si>
+    <t>EK9</t>
+  </si>
+  <si>
+    <t>Z18</t>
+  </si>
+  <si>
+    <t>Z20…Z22</t>
+  </si>
+  <si>
+    <t>EK10</t>
+  </si>
+  <si>
+    <t>Z21</t>
+  </si>
+  <si>
+    <t>SmartRules String SmartRules_StringRangeSpaces(String d)</t>
+  </si>
+  <si>
+    <t>EK11</t>
+  </si>
+  <si>
+    <t>Test SmartRules_StringRangeSpaces</t>
+  </si>
+  <si>
+    <t>&lt;A1</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>EK12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;  A3</t>
+  </si>
+  <si>
+    <t>&lt;=  A5</t>
+  </si>
+  <si>
+    <t>EK15</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>EK14</t>
+  </si>
+  <si>
+    <t>SmartRules String SmartRules_StringRangeSpaces2(String d)</t>
+  </si>
+  <si>
+    <t>Test SmartRules_StringRangeSpaces2</t>
+  </si>
+  <si>
+    <t>&gt;Z999</t>
+  </si>
+  <si>
+    <t>Z1000</t>
+  </si>
+  <si>
+    <t>&gt;  Z998</t>
+  </si>
+  <si>
+    <t>EK16</t>
+  </si>
+  <si>
+    <t>Z999</t>
+  </si>
+  <si>
+    <t>&gt;=   Z996</t>
+  </si>
+  <si>
+    <t>EK18</t>
+  </si>
+  <si>
+    <t>Z996</t>
+  </si>
+  <si>
+    <t>EK19</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>EK20</t>
+  </si>
+  <si>
+    <t>&gt;  A9  &lt;  A11</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>EK21</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>EK22</t>
+  </si>
+  <si>
+    <t>&gt;A6 &lt;A8</t>
+  </si>
+  <si>
+    <t>&gt;=A12 &lt;A13</t>
+  </si>
+  <si>
+    <t>&gt;=  A14 &lt;  A15</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>&gt;A16 &lt;=A17</t>
+  </si>
+  <si>
+    <t>EK23</t>
+  </si>
+  <si>
+    <t>EK24</t>
+  </si>
+  <si>
+    <t>A17</t>
+  </si>
+  <si>
+    <t>&gt;  A18 &lt;=  A19</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>&gt;=A20 &lt;=A20</t>
+  </si>
+  <si>
+    <t>EK25</t>
+  </si>
+  <si>
+    <t>A20</t>
+  </si>
+  <si>
+    <t>&gt;=  A21 &lt;=  A21</t>
+  </si>
+  <si>
+    <t>EK26</t>
+  </si>
+  <si>
+    <t>A21</t>
+  </si>
+  <si>
+    <t>more than  A22</t>
+  </si>
+  <si>
+    <t>EK27</t>
+  </si>
+  <si>
+    <t>A23</t>
+  </si>
+  <si>
+    <t>EK28</t>
+  </si>
+  <si>
+    <t>Z99</t>
+  </si>
+  <si>
+    <t>less than  Z100</t>
+  </si>
+  <si>
+    <t>* add rule and test test for &lt;=A4 after fix EPBDS-8705</t>
+  </si>
+  <si>
+    <t>* add rule and test test for &gt;=Z997 after fix EPBDS-8705</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -453,8 +704,131 @@
       <color indexed="8"/>
       <name val="&quot;Franklin Gothik Book&quot;"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="20"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="23"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color indexed="54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color indexed="54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="62"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="60"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="63"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color indexed="54"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,8 +879,94 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="27"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="47"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="44"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="53"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="62"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -566,11 +1026,130 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="23"/>
+      </left>
+      <right style="thin">
+        <color indexed="23"/>
+      </right>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="63"/>
+      </left>
+      <right style="double">
+        <color indexed="63"/>
+      </right>
+      <top style="double">
+        <color indexed="63"/>
+      </top>
+      <bottom style="double">
+        <color indexed="63"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="49"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="44"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="44"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="52"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="63"/>
+      </left>
+      <right style="thin">
+        <color indexed="63"/>
+      </right>
+      <top style="thin">
+        <color indexed="63"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="63"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="49"/>
+      </top>
+      <bottom style="double">
+        <color indexed="49"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -592,6 +1171,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -604,9 +1206,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal_SmartRules" xfId="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -633,7 +1242,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -904,18 +1513,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A233" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -926,10 +1535,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="3" t="s">
@@ -989,18 +1598,18 @@
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="2" t="s">
@@ -1171,10 +1780,10 @@
       <c r="D36" s="1"/>
     </row>
     <row r="40" spans="2:4">
-      <c r="B40" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C40" s="11"/>
+      <c r="B40" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" s="20"/>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="3" t="s">
@@ -1241,11 +1850,11 @@
       </c>
     </row>
     <row r="52" spans="2:4">
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
     </row>
     <row r="53" spans="2:4">
       <c r="B53" s="2" t="s">
@@ -1435,10 +2044,10 @@
       <c r="D73" s="1"/>
     </row>
     <row r="77" spans="2:4">
-      <c r="B77" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="C77" s="11"/>
+      <c r="B77" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C77" s="20"/>
     </row>
     <row r="78" spans="2:4">
       <c r="B78" s="3" t="s">
@@ -1490,7 +2099,7 @@
     </row>
     <row r="84" spans="2:4">
       <c r="B84" s="6" t="s">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>4</v>
@@ -1498,18 +2107,18 @@
     </row>
     <row r="85" spans="2:4">
       <c r="B85" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="89" spans="2:4">
-      <c r="B89" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C89" s="11"/>
-      <c r="D89" s="11"/>
+      <c r="B89" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C89" s="20"/>
+      <c r="D89" s="20"/>
     </row>
     <row r="90" spans="2:4">
       <c r="B90" s="2" t="s">
@@ -1568,7 +2177,7 @@
     <row r="96" spans="2:4">
       <c r="B96" s="1"/>
       <c r="C96" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>2</v>
@@ -1577,7 +2186,7 @@
     <row r="97" spans="2:4">
       <c r="B97" s="1"/>
       <c r="C97" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>3</v>
@@ -1586,7 +2195,7 @@
     <row r="98" spans="2:4">
       <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>3</v>
@@ -1595,7 +2204,7 @@
     <row r="99" spans="2:4">
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>4</v>
@@ -1604,7 +2213,7 @@
     <row r="100" spans="2:4">
       <c r="B100" s="1"/>
       <c r="C100" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>3</v>
@@ -1613,7 +2222,7 @@
     <row r="101" spans="2:4">
       <c r="B101" s="1"/>
       <c r="C101" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>4</v>
@@ -1622,7 +2231,7 @@
     <row r="102" spans="2:4">
       <c r="B102" s="1"/>
       <c r="C102" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>13</v>
@@ -1631,14 +2240,14 @@
     <row r="103" spans="2:4">
       <c r="B103" s="1"/>
       <c r="C103" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D103" s="1"/>
     </row>
     <row r="104" spans="2:4">
       <c r="B104" s="1"/>
       <c r="C104" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>13</v>
@@ -1647,15 +2256,15 @@
     <row r="105" spans="2:4">
       <c r="B105" s="1"/>
       <c r="C105" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D105" s="1"/>
     </row>
     <row r="109" spans="2:4">
-      <c r="B109" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C109" s="11"/>
+      <c r="B109" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C109" s="20"/>
     </row>
     <row r="110" spans="2:4">
       <c r="B110" s="3" t="s">
@@ -1691,7 +2300,7 @@
     </row>
     <row r="114" spans="2:4">
       <c r="B114" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>2</v>
@@ -1699,7 +2308,7 @@
     </row>
     <row r="115" spans="2:4">
       <c r="B115" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>3</v>
@@ -1707,7 +2316,7 @@
     </row>
     <row r="116" spans="2:4">
       <c r="B116" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>4</v>
@@ -1715,18 +2324,18 @@
     </row>
     <row r="117" spans="2:4">
       <c r="B117" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="120" spans="2:4">
-      <c r="B120" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C120" s="11"/>
-      <c r="D120" s="11"/>
+      <c r="B120" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C120" s="20"/>
+      <c r="D120" s="20"/>
     </row>
     <row r="121" spans="2:4">
       <c r="B121" s="2" t="s">
@@ -1785,7 +2394,7 @@
     <row r="127" spans="2:4">
       <c r="B127" s="1"/>
       <c r="C127" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>2</v>
@@ -1794,7 +2403,7 @@
     <row r="128" spans="2:4">
       <c r="B128" s="1"/>
       <c r="C128" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>3</v>
@@ -1803,7 +2412,7 @@
     <row r="129" spans="2:4">
       <c r="B129" s="1"/>
       <c r="C129" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>3</v>
@@ -1812,7 +2421,7 @@
     <row r="130" spans="2:4">
       <c r="B130" s="1"/>
       <c r="C130" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>4</v>
@@ -1821,7 +2430,7 @@
     <row r="131" spans="2:4">
       <c r="B131" s="1"/>
       <c r="C131" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>3</v>
@@ -1830,7 +2439,7 @@
     <row r="132" spans="2:4">
       <c r="B132" s="1"/>
       <c r="C132" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>4</v>
@@ -1839,7 +2448,7 @@
     <row r="133" spans="2:4">
       <c r="B133" s="1"/>
       <c r="C133" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>13</v>
@@ -1848,14 +2457,14 @@
     <row r="134" spans="2:4">
       <c r="B134" s="1"/>
       <c r="C134" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D134" s="1"/>
     </row>
     <row r="135" spans="2:4">
       <c r="B135" s="1"/>
       <c r="C135" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>13</v>
@@ -1864,15 +2473,15 @@
     <row r="136" spans="2:4">
       <c r="B136" s="1"/>
       <c r="C136" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D136" s="1"/>
     </row>
     <row r="140" spans="2:4">
-      <c r="B140" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C140" s="11"/>
+      <c r="B140" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C140" s="20"/>
     </row>
     <row r="141" spans="2:4">
       <c r="B141" s="3" t="s">
@@ -1908,7 +2517,7 @@
     </row>
     <row r="145" spans="2:4">
       <c r="B145" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C145" s="7" t="s">
         <v>2</v>
@@ -1916,7 +2525,7 @@
     </row>
     <row r="146" spans="2:4">
       <c r="B146" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>3</v>
@@ -1924,7 +2533,7 @@
     </row>
     <row r="147" spans="2:4">
       <c r="B147" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C147" s="7" t="s">
         <v>4</v>
@@ -1932,18 +2541,18 @@
     </row>
     <row r="148" spans="2:4">
       <c r="B148" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C148" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="151" spans="2:4">
-      <c r="B151" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C151" s="11"/>
-      <c r="D151" s="11"/>
+      <c r="B151" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C151" s="20"/>
+      <c r="D151" s="20"/>
     </row>
     <row r="152" spans="2:4">
       <c r="B152" s="2" t="s">
@@ -2002,7 +2611,7 @@
     <row r="158" spans="2:4">
       <c r="B158" s="1"/>
       <c r="C158" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>2</v>
@@ -2011,7 +2620,7 @@
     <row r="159" spans="2:4">
       <c r="B159" s="1"/>
       <c r="C159" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>3</v>
@@ -2020,7 +2629,7 @@
     <row r="160" spans="2:4">
       <c r="B160" s="1"/>
       <c r="C160" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>3</v>
@@ -2029,7 +2638,7 @@
     <row r="161" spans="2:4">
       <c r="B161" s="1"/>
       <c r="C161" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D161" s="1" t="s">
         <v>4</v>
@@ -2038,7 +2647,7 @@
     <row r="162" spans="2:4">
       <c r="B162" s="1"/>
       <c r="C162" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D162" s="1" t="s">
         <v>3</v>
@@ -2047,7 +2656,7 @@
     <row r="163" spans="2:4">
       <c r="B163" s="1"/>
       <c r="C163" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>4</v>
@@ -2056,7 +2665,7 @@
     <row r="164" spans="2:4">
       <c r="B164" s="1"/>
       <c r="C164" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>13</v>
@@ -2065,14 +2674,14 @@
     <row r="165" spans="2:4">
       <c r="B165" s="1"/>
       <c r="C165" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D165" s="1"/>
     </row>
     <row r="166" spans="2:4">
       <c r="B166" s="1"/>
       <c r="C166" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>13</v>
@@ -2081,15 +2690,15 @@
     <row r="167" spans="2:4">
       <c r="B167" s="1"/>
       <c r="C167" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D167" s="1"/>
     </row>
     <row r="172" spans="2:4">
-      <c r="B172" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C172" s="11"/>
+      <c r="B172" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C172" s="20"/>
     </row>
     <row r="173" spans="2:4">
       <c r="B173" s="3" t="s">
@@ -2125,7 +2734,7 @@
     </row>
     <row r="177" spans="2:4">
       <c r="B177" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C177" s="7" t="s">
         <v>2</v>
@@ -2133,7 +2742,7 @@
     </row>
     <row r="178" spans="2:4">
       <c r="B178" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C178" s="7" t="s">
         <v>3</v>
@@ -2141,7 +2750,7 @@
     </row>
     <row r="179" spans="2:4">
       <c r="B179" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C179" s="7" t="s">
         <v>4</v>
@@ -2149,18 +2758,18 @@
     </row>
     <row r="180" spans="2:4">
       <c r="B180" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C180" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="183" spans="2:4">
-      <c r="B183" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C183" s="11"/>
-      <c r="D183" s="11"/>
+      <c r="B183" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C183" s="20"/>
+      <c r="D183" s="20"/>
     </row>
     <row r="184" spans="2:4">
       <c r="B184" s="2" t="s">
@@ -2221,7 +2830,7 @@
     <row r="190" spans="2:4">
       <c r="B190" s="1"/>
       <c r="C190" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>3</v>
@@ -2239,7 +2848,7 @@
     <row r="192" spans="2:4">
       <c r="B192" s="1"/>
       <c r="C192" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D192" s="1" t="s">
         <v>3</v>
@@ -2248,7 +2857,7 @@
     <row r="193" spans="2:4">
       <c r="B193" s="1"/>
       <c r="C193" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D193" s="1" t="s">
         <v>3</v>
@@ -2257,14 +2866,14 @@
     <row r="194" spans="2:4">
       <c r="B194" s="1"/>
       <c r="C194" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D194" s="1"/>
     </row>
     <row r="195" spans="2:4">
       <c r="B195" s="1"/>
       <c r="C195" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D195" s="1"/>
     </row>
@@ -2353,10 +2962,10 @@
       </c>
     </row>
     <row r="209" spans="2:4">
-      <c r="B209" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C209" s="11"/>
+      <c r="B209" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C209" s="20"/>
     </row>
     <row r="210" spans="2:4">
       <c r="B210" s="3" t="s">
@@ -2392,7 +3001,7 @@
     </row>
     <row r="214" spans="2:4">
       <c r="B214" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C214" s="7" t="s">
         <v>2</v>
@@ -2400,7 +3009,7 @@
     </row>
     <row r="215" spans="2:4">
       <c r="B215" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C215" s="7" t="s">
         <v>3</v>
@@ -2408,7 +3017,7 @@
     </row>
     <row r="216" spans="2:4">
       <c r="B216" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C216" s="7" t="s">
         <v>4</v>
@@ -2416,18 +3025,18 @@
     </row>
     <row r="217" spans="2:4">
       <c r="B217" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C217" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="220" spans="2:4">
-      <c r="B220" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C220" s="11"/>
-      <c r="D220" s="11"/>
+      <c r="B220" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C220" s="20"/>
+      <c r="D220" s="20"/>
     </row>
     <row r="221" spans="2:4">
       <c r="B221" s="2" t="s">
@@ -2488,7 +3097,7 @@
     <row r="227" spans="2:4">
       <c r="B227" s="1"/>
       <c r="C227" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D227" s="1" t="s">
         <v>3</v>
@@ -2506,7 +3115,7 @@
     <row r="229" spans="2:4">
       <c r="B229" s="1"/>
       <c r="C229" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D229" s="1" t="s">
         <v>3</v>
@@ -2515,7 +3124,7 @@
     <row r="230" spans="2:4">
       <c r="B230" s="1"/>
       <c r="C230" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D230" s="1" t="s">
         <v>3</v>
@@ -2524,14 +3133,14 @@
     <row r="231" spans="2:4">
       <c r="B231" s="1"/>
       <c r="C231" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D231" s="1"/>
     </row>
     <row r="232" spans="2:4">
       <c r="B232" s="1"/>
       <c r="C232" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D232" s="1"/>
     </row>
@@ -2620,10 +3229,10 @@
       </c>
     </row>
     <row r="245" spans="2:4">
-      <c r="B245" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C245" s="11"/>
+      <c r="B245" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C245" s="20"/>
     </row>
     <row r="246" spans="2:4">
       <c r="B246" s="3" t="s">
@@ -2659,18 +3268,18 @@
     </row>
     <row r="250" spans="2:4">
       <c r="B250" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C250" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="254" spans="2:4">
-      <c r="B254" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C254" s="11"/>
-      <c r="D254" s="11"/>
+      <c r="B254" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C254" s="20"/>
+      <c r="D254" s="20"/>
     </row>
     <row r="255" spans="2:4">
       <c r="B255" s="2" t="s">
@@ -2727,7 +3336,7 @@
     <row r="261" spans="2:4">
       <c r="B261" s="1"/>
       <c r="C261" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D261" s="1" t="s">
         <v>2</v>
@@ -2745,7 +3354,7 @@
     <row r="263" spans="2:4">
       <c r="B263" s="1"/>
       <c r="C263" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D263" s="1" t="s">
         <v>2</v>
@@ -2754,7 +3363,7 @@
     <row r="264" spans="2:4">
       <c r="B264" s="1"/>
       <c r="C264" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D264" s="1" t="s">
         <v>2</v>
@@ -2763,7 +3372,7 @@
     <row r="265" spans="2:4">
       <c r="B265" s="1"/>
       <c r="C265" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D265" s="1" t="s">
         <v>2</v>
@@ -2772,7 +3381,7 @@
     <row r="266" spans="2:4">
       <c r="B266" s="1"/>
       <c r="C266" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D266" s="1" t="s">
         <v>2</v>
@@ -2893,307 +3502,811 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B3:D36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:N58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="29.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="40.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="32.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="27.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4">
-      <c r="B3" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="11"/>
-    </row>
-    <row r="4" spans="2:4">
+    <row r="3" spans="2:13">
+      <c r="B3" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="H3" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="I3" s="20"/>
+      <c r="L3" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="M3" s="20"/>
+    </row>
+    <row r="4" spans="2:13">
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:4">
+      <c r="H4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13">
       <c r="B5" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="H5" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="B6" s="6" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
+      <c r="H6" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="15.75">
       <c r="B7" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="2:4">
+      <c r="H7" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="15.75">
       <c r="B8" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="2:4">
+      <c r="H8" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="15.75">
       <c r="B9" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="2:4">
+      <c r="H9" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="15.75">
       <c r="B10" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="2" t="s">
+      <c r="H10" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+    </row>
+    <row r="11" spans="2:13" ht="16.5" customHeight="1">
+      <c r="B11" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+    </row>
+    <row r="12" spans="2:13" ht="16.5" customHeight="1">
+      <c r="B12" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+    </row>
+    <row r="13" spans="2:13" ht="15.75">
+      <c r="B13" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+    </row>
+    <row r="14" spans="2:13" ht="15.75">
+      <c r="B14" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+    </row>
+    <row r="15" spans="2:13" ht="15.75">
+      <c r="B15" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+    </row>
+    <row r="16" spans="2:13" ht="15.75">
+      <c r="B16" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+    </row>
+    <row r="17" spans="2:14" ht="15.75">
+      <c r="B17" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+    </row>
+    <row r="18" spans="2:14" ht="15.75">
+      <c r="B18" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+    </row>
+    <row r="19" spans="2:14" ht="15.75">
+      <c r="B19" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+    </row>
+    <row r="20" spans="2:14" ht="15.75">
+      <c r="B20" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H20" s="16"/>
+      <c r="I20" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+    </row>
+    <row r="21" spans="2:14" ht="15.75">
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="L21" s="17" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+    </row>
+    <row r="25" spans="2:14">
+      <c r="B25" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="H25" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="L25" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+    </row>
+    <row r="26" spans="2:14">
+      <c r="B26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="J26" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="1" t="s">
+      <c r="L26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14">
+      <c r="B27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14">
+      <c r="B28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="L28" s="1"/>
+      <c r="M28" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="N28" s="12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14">
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4">
+      <c r="H29" s="1"/>
+      <c r="I29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14">
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4">
+        <v>2</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14">
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
+        <v>2</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14">
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4">
+        <v>2</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4">
+        <v>3</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10">
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4">
+        <v>3</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10">
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4">
+        <v>4</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10">
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>97</v>
+        <v>3</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="2:10">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10">
+      <c r="B45" s="1"/>
+      <c r="C45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10">
+      <c r="B46" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10">
+      <c r="B48" s="1"/>
+      <c r="C48" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="12"/>
+      <c r="C49" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="B50" s="1"/>
+      <c r="C50" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="1"/>
+      <c r="C51" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="1"/>
+      <c r="C52" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" s="1"/>
+      <c r="C53" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" s="1"/>
+      <c r="C54" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="C55" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4">
+      <c r="C56" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="C57" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4">
+      <c r="C58" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L25:N25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3204,10 +4317,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
-      <c r="B2" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="11"/>
+      <c r="B2" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="4" t="s">
@@ -3219,18 +4332,18 @@
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -3251,7 +4364,7 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -3259,18 +4372,18 @@
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="B14" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="2" t="s">
@@ -3329,7 +4442,7 @@
     <row r="21" spans="2:4">
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>2</v>
@@ -3338,7 +4451,7 @@
     <row r="22" spans="2:4">
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>3</v>
@@ -3347,7 +4460,7 @@
     <row r="23" spans="2:4">
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>3</v>
@@ -3356,7 +4469,7 @@
     <row r="24" spans="2:4">
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>4</v>
@@ -3365,7 +4478,7 @@
     <row r="25" spans="2:4">
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>3</v>
@@ -3374,7 +4487,7 @@
     <row r="26" spans="2:4">
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>4</v>
@@ -3383,7 +4496,7 @@
     <row r="27" spans="2:4">
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>13</v>
@@ -3392,14 +4505,14 @@
     <row r="28" spans="2:4">
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>13</v>
@@ -3408,17 +4521,17 @@
     <row r="30" spans="2:4">
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="32" spans="2:4">
@@ -3427,40 +4540,40 @@
         <v>22</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="2:4">
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>2</v>
@@ -3469,10 +4582,10 @@
     <row r="37" spans="2:4">
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -3485,106 +4598,106 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:12">
-      <c r="B4" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="G4" s="11" t="s">
+      <c r="B4" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
+      <c r="C4" s="20"/>
+      <c r="G4" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
     </row>
     <row r="5" spans="2:12">
       <c r="B5" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="G5" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="6" spans="2:12">
       <c r="B6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="7" spans="2:12">
       <c r="B7" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J7" s="1" t="b">
         <v>0</v>
@@ -3598,19 +4711,19 @@
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J8" s="1" t="b">
         <v>0</v>
@@ -3624,39 +4737,39 @@
     </row>
     <row r="9" spans="2:12">
       <c r="B9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
+      <c r="B15" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
     </row>
     <row r="16" spans="2:12">
       <c r="B16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-8705 Add test for "<=a" and ">=a"
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Ranges_StringRange.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Ranges_StringRange.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="223">
   <si>
     <t>d</t>
   </si>
@@ -675,17 +675,29 @@
     <t>less than  Z100</t>
   </si>
   <si>
-    <t>* add rule and test test for &lt;=A4 after fix EPBDS-8705</t>
-  </si>
-  <si>
-    <t>* add rule and test test for &gt;=Z997 after fix EPBDS-8705</t>
+    <t xml:space="preserve"> &lt;=A4</t>
+  </si>
+  <si>
+    <t>EK29</t>
+  </si>
+  <si>
+    <t>&gt;=Z997</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>EK30</t>
+  </si>
+  <si>
+    <t>Z997</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -718,117 +730,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="20"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="52"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color indexed="23"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="17"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color indexed="54"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color indexed="54"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="54"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="62"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="52"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="60"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="63"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color indexed="54"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color indexed="8"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -879,94 +786,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="27"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="47"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="26"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="31"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="44"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="22"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="43"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="49"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="53"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="62"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="45"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1039,108 +860,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="23"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="23"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="23"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="23"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="63"/>
-      </left>
-      <right style="double">
-        <color indexed="63"/>
-      </right>
-      <top style="double">
-        <color indexed="63"/>
-      </top>
-      <bottom style="double">
-        <color indexed="63"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color indexed="49"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color indexed="44"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="44"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color indexed="52"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="22"/>
-      </left>
-      <right style="thin">
-        <color indexed="22"/>
-      </right>
-      <top style="thin">
-        <color indexed="22"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="63"/>
-      </left>
-      <right style="thin">
-        <color indexed="63"/>
-      </right>
-      <top style="thin">
-        <color indexed="63"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="63"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="49"/>
-      </top>
-      <bottom style="double">
-        <color indexed="49"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1149,7 +878,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1185,13 +914,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1206,10 +932,34 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1513,7 +1263,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1535,10 +1285,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="19"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="3" t="s">
@@ -1605,11 +1355,11 @@
       </c>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="2" t="s">
@@ -1780,10 +1530,10 @@
       <c r="D36" s="1"/>
     </row>
     <row r="40" spans="2:4">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="20"/>
+      <c r="C40" s="19"/>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="3" t="s">
@@ -1850,11 +1600,11 @@
       </c>
     </row>
     <row r="52" spans="2:4">
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
     </row>
     <row r="53" spans="2:4">
       <c r="B53" s="2" t="s">
@@ -2044,10 +1794,10 @@
       <c r="D73" s="1"/>
     </row>
     <row r="77" spans="2:4">
-      <c r="B77" s="20" t="s">
+      <c r="B77" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="C77" s="20"/>
+      <c r="C77" s="19"/>
     </row>
     <row r="78" spans="2:4">
       <c r="B78" s="3" t="s">
@@ -2114,11 +1864,11 @@
       </c>
     </row>
     <row r="89" spans="2:4">
-      <c r="B89" s="20" t="s">
+      <c r="B89" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C89" s="20"/>
-      <c r="D89" s="20"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="19"/>
     </row>
     <row r="90" spans="2:4">
       <c r="B90" s="2" t="s">
@@ -2261,10 +2011,10 @@
       <c r="D105" s="1"/>
     </row>
     <row r="109" spans="2:4">
-      <c r="B109" s="20" t="s">
+      <c r="B109" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C109" s="20"/>
+      <c r="C109" s="19"/>
     </row>
     <row r="110" spans="2:4">
       <c r="B110" s="3" t="s">
@@ -2331,11 +2081,11 @@
       </c>
     </row>
     <row r="120" spans="2:4">
-      <c r="B120" s="20" t="s">
+      <c r="B120" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C120" s="20"/>
-      <c r="D120" s="20"/>
+      <c r="C120" s="19"/>
+      <c r="D120" s="19"/>
     </row>
     <row r="121" spans="2:4">
       <c r="B121" s="2" t="s">
@@ -2478,10 +2228,10 @@
       <c r="D136" s="1"/>
     </row>
     <row r="140" spans="2:4">
-      <c r="B140" s="20" t="s">
+      <c r="B140" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C140" s="20"/>
+      <c r="C140" s="19"/>
     </row>
     <row r="141" spans="2:4">
       <c r="B141" s="3" t="s">
@@ -2548,11 +2298,11 @@
       </c>
     </row>
     <row r="151" spans="2:4">
-      <c r="B151" s="20" t="s">
+      <c r="B151" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="C151" s="20"/>
-      <c r="D151" s="20"/>
+      <c r="C151" s="19"/>
+      <c r="D151" s="19"/>
     </row>
     <row r="152" spans="2:4">
       <c r="B152" s="2" t="s">
@@ -2695,10 +2445,10 @@
       <c r="D167" s="1"/>
     </row>
     <row r="172" spans="2:4">
-      <c r="B172" s="20" t="s">
+      <c r="B172" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C172" s="20"/>
+      <c r="C172" s="19"/>
     </row>
     <row r="173" spans="2:4">
       <c r="B173" s="3" t="s">
@@ -2765,11 +2515,11 @@
       </c>
     </row>
     <row r="183" spans="2:4">
-      <c r="B183" s="20" t="s">
+      <c r="B183" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C183" s="20"/>
-      <c r="D183" s="20"/>
+      <c r="C183" s="19"/>
+      <c r="D183" s="19"/>
     </row>
     <row r="184" spans="2:4">
       <c r="B184" s="2" t="s">
@@ -2962,10 +2712,10 @@
       </c>
     </row>
     <row r="209" spans="2:4">
-      <c r="B209" s="20" t="s">
+      <c r="B209" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C209" s="20"/>
+      <c r="C209" s="19"/>
     </row>
     <row r="210" spans="2:4">
       <c r="B210" s="3" t="s">
@@ -3032,11 +2782,11 @@
       </c>
     </row>
     <row r="220" spans="2:4">
-      <c r="B220" s="20" t="s">
+      <c r="B220" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C220" s="20"/>
-      <c r="D220" s="20"/>
+      <c r="C220" s="19"/>
+      <c r="D220" s="19"/>
     </row>
     <row r="221" spans="2:4">
       <c r="B221" s="2" t="s">
@@ -3229,10 +2979,10 @@
       </c>
     </row>
     <row r="245" spans="2:4">
-      <c r="B245" s="20" t="s">
+      <c r="B245" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C245" s="20"/>
+      <c r="C245" s="19"/>
     </row>
     <row r="246" spans="2:4">
       <c r="B246" s="3" t="s">
@@ -3275,11 +3025,11 @@
       </c>
     </row>
     <row r="254" spans="2:4">
-      <c r="B254" s="20" t="s">
+      <c r="B254" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C254" s="20"/>
-      <c r="D254" s="20"/>
+      <c r="C254" s="19"/>
+      <c r="D254" s="19"/>
     </row>
     <row r="255" spans="2:4">
       <c r="B255" s="2" t="s">
@@ -3505,8 +3255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3521,18 +3271,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="H3" s="20" t="s">
+      <c r="C3" s="19"/>
+      <c r="H3" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="L3" s="20" t="s">
+      <c r="I3" s="26"/>
+      <c r="L3" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="M3" s="20"/>
+      <c r="M3" s="19"/>
     </row>
     <row r="4" spans="2:13">
       <c r="B4" s="4" t="s">
@@ -3541,10 +3291,10 @@
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="28" t="s">
         <v>1</v>
       </c>
       <c r="L4" s="4" t="s">
@@ -3561,10 +3311,10 @@
       <c r="C5" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="30" t="s">
         <v>167</v>
       </c>
       <c r="L5" s="6" t="s">
@@ -3581,10 +3331,10 @@
       <c r="C6" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="30" t="s">
         <v>171</v>
       </c>
       <c r="L6" s="6" t="s">
@@ -3601,17 +3351,17 @@
       <c r="C7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>176</v>
+      <c r="H7" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>218</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>184</v>
+        <v>219</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>185</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="15.75">
@@ -3621,17 +3371,17 @@
       <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>187</v>
+      <c r="H8" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>176</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="15.75">
@@ -3641,11 +3391,11 @@
       <c r="C9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>189</v>
+      <c r="H9" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>187</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>216</v>
@@ -3661,14 +3411,18 @@
       <c r="C10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
+      <c r="H10" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="11" spans="2:13" ht="16.5" customHeight="1">
       <c r="B11" s="6" t="s">
@@ -3677,14 +3431,14 @@
       <c r="C11" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="H11" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
+      <c r="H11" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
     </row>
     <row r="12" spans="2:13" ht="16.5" customHeight="1">
       <c r="B12" s="6" t="s">
@@ -3693,14 +3447,14 @@
       <c r="C12" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H12" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
+      <c r="H12" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
     </row>
     <row r="13" spans="2:13" ht="15.75">
       <c r="B13" s="6" t="s">
@@ -3709,14 +3463,14 @@
       <c r="C13" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="H13" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
+      <c r="H13" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
     </row>
     <row r="14" spans="2:13" ht="15.75">
       <c r="B14" s="6" t="s">
@@ -3725,14 +3479,14 @@
       <c r="C14" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="H14" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
+      <c r="H14" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
     </row>
     <row r="15" spans="2:13" ht="15.75">
       <c r="B15" s="6" t="s">
@@ -3741,14 +3495,14 @@
       <c r="C15" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="H15" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
+      <c r="H15" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
     </row>
     <row r="16" spans="2:13" ht="15.75">
       <c r="B16" s="6" t="s">
@@ -3757,14 +3511,14 @@
       <c r="C16" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="H16" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="I16" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
+      <c r="H16" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
     </row>
     <row r="17" spans="2:14" ht="15.75">
       <c r="B17" s="6" t="s">
@@ -3773,10 +3527,14 @@
       <c r="C17" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
+      <c r="H17" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
     </row>
     <row r="18" spans="2:14" ht="15.75">
       <c r="B18" s="6" t="s">
@@ -3785,10 +3543,10 @@
       <c r="C18" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
     </row>
     <row r="19" spans="2:14" ht="15.75">
       <c r="B19" s="6" t="s">
@@ -3799,8 +3557,8 @@
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
     </row>
     <row r="20" spans="2:14" ht="15.75">
       <c r="B20" s="6" t="s">
@@ -3809,21 +3567,22 @@
       <c r="C20" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="H20" s="16"/>
-      <c r="I20" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
     </row>
     <row r="21" spans="2:14" ht="15.75">
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="L21" s="17" t="s">
-        <v>218</v>
-      </c>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="33"/>
     </row>
     <row r="22" spans="2:14">
       <c r="B22" s="14"/>
@@ -3834,21 +3593,21 @@
       <c r="C23" s="15"/>
     </row>
     <row r="25" spans="2:14">
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="H25" s="20" t="s">
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="H25" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="L25" s="20" t="s">
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="L25" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
     </row>
     <row r="26" spans="2:14">
       <c r="B26" s="2" t="s">
@@ -4011,6 +3770,12 @@
       <c r="J32" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="M32" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="N32" s="13" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="33" spans="2:10">
       <c r="B33" s="1"/>
@@ -4129,6 +3894,13 @@
       </c>
       <c r="D40" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="H40" s="24"/>
+      <c r="I40" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="J40" s="25" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="2:10">
@@ -4317,10 +4089,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="19"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="4" t="s">
@@ -4379,11 +4151,11 @@
       </c>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="2" t="s">
@@ -4618,18 +4390,18 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:12">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="G4" s="20" t="s">
+      <c r="C4" s="19"/>
+      <c r="G4" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
     </row>
     <row r="5" spans="2:12">
       <c r="B5" s="9" t="s">
@@ -4744,11 +4516,11 @@
       </c>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
     </row>
     <row r="16" spans="2:12">
       <c r="B16" s="1" t="s">

</xml_diff>